<commit_message>
0805~0806 clubs + posts + photos + login popups ...
</commit_message>
<xml_diff>
--- a/팀작업 테이블명세서.xlsx
+++ b/팀작업 테이블명세서.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8085" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="2"/>
+    <workbookView xWindow="9225" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="503">
   <si>
     <t>Null허용</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2145,6 +2145,34 @@
   </si>
   <si>
     <t>Date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pkind</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pcon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>포스트 종류</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>포스트 공개성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(45)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>a, b, c로 이루어져 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">자랑, 후기, 모집으로 이루어져 있다. </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2560,9 +2588,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2570,6 +2595,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3321,15 +3349,15 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
       <c r="J20" s="2">
         <v>1</v>
       </c>
@@ -3516,15 +3544,15 @@
         <v>18</v>
       </c>
       <c r="G26" s="2"/>
-      <c r="J26" s="44" t="s">
+      <c r="J26" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="46"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+      <c r="P26" s="45"/>
       <c r="Q26" t="s">
         <v>218</v>
       </c>
@@ -4386,14 +4414,14 @@
       <c r="A63" s="4"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F65" s="43" t="s">
+      <c r="F65" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="G65" s="43"/>
-      <c r="H65" s="43"/>
-      <c r="I65" s="43"/>
-      <c r="J65" s="43"/>
-      <c r="K65" s="43"/>
+      <c r="G65" s="46"/>
+      <c r="H65" s="46"/>
+      <c r="I65" s="46"/>
+      <c r="J65" s="46"/>
+      <c r="K65" s="46"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="M66" t="s">
@@ -4716,6 +4744,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A33:G33"/>
     <mergeCell ref="J67:P67"/>
     <mergeCell ref="J55:P55"/>
     <mergeCell ref="J18:P18"/>
@@ -4725,11 +4758,6 @@
     <mergeCell ref="A55:G55"/>
     <mergeCell ref="A67:G67"/>
     <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A33:G33"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4769,39 +4797,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="46" t="s">
         <v>226</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="K5" s="9"/>
@@ -7554,12 +7582,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B88:I88"/>
-    <mergeCell ref="K69:R69"/>
-    <mergeCell ref="K53:R53"/>
-    <mergeCell ref="K36:R36"/>
-    <mergeCell ref="K80:R80"/>
-    <mergeCell ref="B80:I80"/>
     <mergeCell ref="B122:I122"/>
     <mergeCell ref="C2:K4"/>
     <mergeCell ref="B7:I7"/>
@@ -7573,6 +7595,12 @@
     <mergeCell ref="K27:R27"/>
     <mergeCell ref="B53:I53"/>
     <mergeCell ref="B69:I69"/>
+    <mergeCell ref="B88:I88"/>
+    <mergeCell ref="K69:R69"/>
+    <mergeCell ref="K53:R53"/>
+    <mergeCell ref="K36:R36"/>
+    <mergeCell ref="K80:R80"/>
+    <mergeCell ref="B80:I80"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7584,8 +7612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101:I101"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R76" sqref="R76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7615,39 +7643,39 @@
         <f ca="1">B2:T134</f>
         <v>0</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="46" t="s">
         <v>226</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="K5" s="9"/>
@@ -9744,8 +9772,8 @@
       <c r="M74" s="27" t="s">
         <v>292</v>
       </c>
-      <c r="N74" s="27" t="s">
-        <v>232</v>
+      <c r="N74" s="21" t="s">
+        <v>500</v>
       </c>
       <c r="O74" s="26"/>
       <c r="P74" s="26"/>
@@ -9807,25 +9835,25 @@
       <c r="H76" s="29"/>
       <c r="I76" s="29"/>
       <c r="J76" s="28"/>
-      <c r="K76" s="26">
-        <v>7</v>
-      </c>
-      <c r="L76" s="27" t="s">
-        <v>406</v>
-      </c>
-      <c r="M76" s="27" t="s">
-        <v>407</v>
-      </c>
-      <c r="N76" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="O76" s="26"/>
-      <c r="P76" s="26"/>
-      <c r="Q76" s="26"/>
-      <c r="R76" s="26"/>
-      <c r="S76" s="28" t="s">
-        <v>358</v>
-      </c>
+      <c r="K76" s="22">
+        <v>6</v>
+      </c>
+      <c r="L76" s="21" t="s">
+        <v>498</v>
+      </c>
+      <c r="M76" s="21" t="s">
+        <v>496</v>
+      </c>
+      <c r="N76" s="21" t="s">
+        <v>500</v>
+      </c>
+      <c r="O76" s="22"/>
+      <c r="P76" s="22"/>
+      <c r="Q76" s="22"/>
+      <c r="R76" s="22" t="s">
+        <v>502</v>
+      </c>
+      <c r="S76" s="28"/>
     </row>
     <row r="77" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B77" s="28"/>
@@ -9837,14 +9865,24 @@
       <c r="H77" s="29"/>
       <c r="I77" s="29"/>
       <c r="J77" s="28"/>
-      <c r="K77" s="28"/>
-      <c r="L77" s="28"/>
-      <c r="M77" s="28"/>
-      <c r="N77" s="28"/>
-      <c r="O77" s="29"/>
-      <c r="P77" s="29"/>
-      <c r="Q77" s="29"/>
-      <c r="R77" s="29"/>
+      <c r="K77" s="22">
+        <v>7</v>
+      </c>
+      <c r="L77" s="21" t="s">
+        <v>499</v>
+      </c>
+      <c r="M77" s="21" t="s">
+        <v>497</v>
+      </c>
+      <c r="N77" s="21" t="s">
+        <v>500</v>
+      </c>
+      <c r="O77" s="22"/>
+      <c r="P77" s="22"/>
+      <c r="Q77" s="22"/>
+      <c r="R77" s="22" t="s">
+        <v>501</v>
+      </c>
       <c r="S77" s="28"/>
     </row>
     <row r="78" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -11429,13 +11467,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B36:I36"/>
-    <mergeCell ref="K36:R36"/>
-    <mergeCell ref="C2:K4"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="K14:R14"/>
-    <mergeCell ref="B27:I27"/>
-    <mergeCell ref="K27:R27"/>
     <mergeCell ref="B140:I140"/>
     <mergeCell ref="B56:I56"/>
     <mergeCell ref="K53:R53"/>
@@ -11448,6 +11479,13 @@
     <mergeCell ref="B111:I111"/>
     <mergeCell ref="B118:I118"/>
     <mergeCell ref="B126:I126"/>
+    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="K36:R36"/>
+    <mergeCell ref="C2:K4"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="K14:R14"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="K27:R27"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>